<commit_message>
For LEAD4.0 first change
</commit_message>
<xml_diff>
--- a/2统计表/T.xlsx
+++ b/2统计表/T.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="14400" windowHeight="12270"/>
+    <workbookView windowWidth="21000" windowHeight="11145"/>
   </bookViews>
   <sheets>
     <sheet name="磨溪016-H1_VDL_20200311(4777-6048" sheetId="1" r:id="rId1"/>
@@ -67,8 +67,8 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="21">
@@ -80,14 +80,56 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10.5"/>
+      <sz val="12"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
       <charset val="134"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -95,53 +137,23 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FF3F3F3F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FFFFFFFF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -155,54 +167,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -216,15 +182,48 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -239,19 +238,145 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -263,25 +388,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -293,25 +406,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -321,110 +422,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="13">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -433,53 +432,16 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
+      <left style="thin">
         <color auto="1"/>
       </left>
-      <right style="medium">
+      <right style="thin">
         <color auto="1"/>
       </right>
-      <top style="medium">
+      <top style="thin">
         <color auto="1"/>
       </top>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color auto="1"/>
-      </right>
-      <top style="medium">
-        <color auto="1"/>
-      </top>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color auto="1"/>
-      </left>
-      <right style="medium">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom style="medium">
+      <bottom style="thin">
         <color auto="1"/>
       </bottom>
       <diagonal/>
@@ -501,6 +463,21 @@
     </border>
     <border>
       <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
@@ -515,6 +492,21 @@
       <diagonal/>
     </border>
     <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
@@ -524,17 +516,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -558,30 +544,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -590,163 +552,154 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="11" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="15" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="22" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="30" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -1070,7 +1023,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="C3:D5"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="4" outlineLevelCol="4"/>
@@ -1092,7 +1045,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" ht="14.25" spans="1:5">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1117,10 +1070,10 @@
         <v>9</v>
       </c>
       <c r="C3" s="1">
-        <v>2043.6</v>
-      </c>
-      <c r="D3" s="2">
-        <v>49</v>
+        <v>2750.47</v>
+      </c>
+      <c r="D3" s="1">
+        <v>54.54</v>
       </c>
       <c r="E3" t="s">
         <v>10</v>
@@ -1133,11 +1086,11 @@
       <c r="B4" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="3">
-        <v>584.5</v>
-      </c>
-      <c r="D4" s="4">
-        <v>14</v>
+      <c r="C4" s="1">
+        <v>760.22</v>
+      </c>
+      <c r="D4" s="1">
+        <v>15.07</v>
       </c>
       <c r="E4" t="s">
         <v>12</v>
@@ -1150,11 +1103,11 @@
       <c r="B5" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="3">
-        <v>1541.9</v>
-      </c>
-      <c r="D5" s="4">
-        <v>37</v>
+      <c r="C5" s="1">
+        <v>1532.31</v>
+      </c>
+      <c r="D5" s="1">
+        <v>30.39</v>
       </c>
       <c r="E5" t="s">
         <v>14</v>

</xml_diff>